<commit_message>
testing: xlsx report testing
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Estimates" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Estimates!$A$1:$K$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Estimates!$A$1:$K$77</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t xml:space="preserve">Task / Subtask</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve">Min (P=95%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max (P=95%)</t>
   </si>
 </sst>
 </file>
@@ -3068,7 +3071,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B87" s="20"/>
       <c r="C87" s="21" t="n">

</xml_diff>

<commit_message>
MVP column, option, total row
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>Task / Subtask</t>
   </si>
@@ -24,6 +24,9 @@
     <t>Filter</t>
   </si>
   <si>
+    <t>MVP</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -229,6 +232,9 @@
   </si>
   <si>
     <t xml:space="preserve">  - test</t>
+  </si>
+  <si>
+    <t>Total (MVP)</t>
   </si>
   <si>
     <t>Standard deviation</t>
@@ -720,7 +726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,50 +758,52 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s"/>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="5" t="s"/>
       <c r="I1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s"/>
       <c r="C2" s="6" t="s"/>
       <c r="D2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="9">
         <f>E3+E12+E17+E19</f>
@@ -816,7 +824,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="11" t="s"/>
       <c r="C3" s="10" t="s"/>
@@ -840,12 +848,14 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s"/>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D4" s="3" t="s"/>
       <c r="E4" s="14">
         <f>E5</f>
@@ -875,7 +885,7 @@
     </row>
     <row hidden="1" r="5" spans="1:16">
       <c r="A5" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="16" t="n">
         <v>0</v>
@@ -897,12 +907,14 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s"/>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D6" s="3" t="s"/>
       <c r="E6" s="14">
         <f>E7</f>
@@ -932,7 +944,7 @@
     </row>
     <row hidden="1" r="7" spans="1:16">
       <c r="A7" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="16" t="n">
         <v>0</v>
@@ -954,12 +966,14 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s"/>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D8" s="3" t="s"/>
       <c r="E8" s="14">
         <f>E9</f>
@@ -989,7 +1003,7 @@
     </row>
     <row hidden="1" r="9" spans="1:16">
       <c r="A9" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="16" t="n">
         <v>0</v>
@@ -1011,12 +1025,14 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s"/>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D10" s="3" t="s"/>
       <c r="E10" s="14">
         <f>E11</f>
@@ -1046,7 +1062,7 @@
     </row>
     <row hidden="1" r="11" spans="1:16">
       <c r="A11" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="16" t="n">
         <v>0</v>
@@ -1068,7 +1084,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="11" t="s"/>
       <c r="C12" s="10" t="s"/>
@@ -1092,12 +1108,14 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s"/>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D13" s="3" t="s"/>
       <c r="E13" s="14">
         <f>E14</f>
@@ -1127,7 +1145,7 @@
     </row>
     <row hidden="1" r="14" spans="1:16">
       <c r="A14" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="16" t="n">
         <v>0</v>
@@ -1149,12 +1167,14 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s"/>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D15" s="3" t="s"/>
       <c r="E15" s="14">
         <f>E16</f>
@@ -1184,7 +1204,7 @@
     </row>
     <row hidden="1" r="16" spans="1:16">
       <c r="A16" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="16" t="n">
         <v>0</v>
@@ -1206,12 +1226,14 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s"/>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D17" s="3" t="s"/>
       <c r="E17" s="14">
         <f>E18</f>
@@ -1241,7 +1263,7 @@
     </row>
     <row hidden="1" r="18" spans="1:16">
       <c r="A18" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="16" t="n">
         <v>0</v>
@@ -1263,12 +1285,14 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s"/>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D19" s="3" t="s"/>
       <c r="E19" s="14">
         <f>E20</f>
@@ -1298,7 +1322,7 @@
     </row>
     <row hidden="1" r="20" spans="1:16">
       <c r="A20" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="16" t="n">
         <v>0</v>
@@ -1320,12 +1344,12 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="7" t="s"/>
       <c r="C21" s="6" t="s"/>
       <c r="D21" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="9">
         <f>E22+E29+E32</f>
@@ -1346,12 +1370,12 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="11" t="s"/>
       <c r="C22" s="10" t="s"/>
       <c r="D22" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" s="13">
         <f>E23+E25+E27</f>
@@ -1372,12 +1396,14 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s"/>
+      <c r="C23" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D23" s="3" t="s"/>
       <c r="E23" s="14">
         <f>E24</f>
@@ -1407,7 +1433,7 @@
     </row>
     <row hidden="1" r="24" spans="1:16">
       <c r="A24" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="16" t="n">
         <v>0</v>
@@ -1429,12 +1455,14 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s"/>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D25" s="3" t="s"/>
       <c r="E25" s="14">
         <f>E26</f>
@@ -1464,7 +1492,7 @@
     </row>
     <row hidden="1" r="26" spans="1:16">
       <c r="A26" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="16" t="n">
         <v>0</v>
@@ -1486,12 +1514,14 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s"/>
+      <c r="C27" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D27" s="3" t="s"/>
       <c r="E27" s="14">
         <f>E28</f>
@@ -1521,7 +1551,7 @@
     </row>
     <row hidden="1" r="28" spans="1:16">
       <c r="A28" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" s="16" t="n">
         <v>0</v>
@@ -1543,12 +1573,14 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s"/>
+      <c r="C29" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D29" s="3" t="s"/>
       <c r="E29" s="14">
         <f>E30+E31</f>
@@ -1578,7 +1610,7 @@
     </row>
     <row hidden="1" r="30" spans="1:16">
       <c r="A30" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" s="16" t="n">
         <v>0</v>
@@ -1600,7 +1632,7 @@
     </row>
     <row hidden="1" r="31" spans="1:16">
       <c r="A31" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="16" t="n">
         <v>0</v>
@@ -1622,12 +1654,14 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s"/>
+      <c r="C32" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D32" s="3" t="s"/>
       <c r="E32" s="14">
         <f>E33+E34</f>
@@ -1657,7 +1691,7 @@
     </row>
     <row hidden="1" r="33" spans="1:16">
       <c r="A33" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B33" s="16" t="n">
         <v>0</v>
@@ -1679,7 +1713,7 @@
     </row>
     <row hidden="1" r="34" spans="1:16">
       <c r="A34" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="16" t="n">
         <v>0</v>
@@ -1701,12 +1735,12 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="7" t="s"/>
       <c r="C35" s="6" t="s"/>
       <c r="D35" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E35" s="9">
         <f>E36+E41+E43+E45+E47</f>
@@ -1727,7 +1761,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" s="11" t="s"/>
       <c r="C36" s="10" t="s"/>
@@ -1751,12 +1785,14 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="1" t="s"/>
+      <c r="C37" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D37" s="3" t="s"/>
       <c r="E37" s="14">
         <f>E38</f>
@@ -1786,7 +1822,7 @@
     </row>
     <row hidden="1" r="38" spans="1:16">
       <c r="A38" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B38" s="16" t="n">
         <v>0</v>
@@ -1808,12 +1844,14 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C39" s="1" t="s"/>
+      <c r="C39" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D39" s="3" t="s"/>
       <c r="E39" s="14">
         <f>E40</f>
@@ -1843,7 +1881,7 @@
     </row>
     <row hidden="1" r="40" spans="1:16">
       <c r="A40" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B40" s="16" t="n">
         <v>0</v>
@@ -1865,12 +1903,14 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s"/>
+      <c r="C41" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D41" s="3" t="s"/>
       <c r="E41" s="14">
         <f>E42</f>
@@ -1900,7 +1940,7 @@
     </row>
     <row hidden="1" r="42" spans="1:16">
       <c r="A42" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="16" t="n">
         <v>0</v>
@@ -1922,12 +1962,14 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="1" t="s"/>
+      <c r="C43" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D43" s="3" t="s"/>
       <c r="E43" s="14">
         <f>E44</f>
@@ -1957,7 +1999,7 @@
     </row>
     <row hidden="1" r="44" spans="1:16">
       <c r="A44" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B44" s="16" t="n">
         <v>0</v>
@@ -1979,12 +2021,14 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s"/>
+      <c r="C45" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D45" s="3" t="s"/>
       <c r="E45" s="14">
         <f>E46</f>
@@ -2014,7 +2058,7 @@
     </row>
     <row hidden="1" r="46" spans="1:16">
       <c r="A46" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B46" s="16" t="n">
         <v>0</v>
@@ -2036,14 +2080,16 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="s"/>
+      <c r="C47" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D47" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E47" s="14">
         <f>E48</f>
@@ -2073,7 +2119,7 @@
     </row>
     <row hidden="1" r="48" spans="1:16">
       <c r="A48" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B48" s="16" t="n">
         <v>0</v>
@@ -2095,12 +2141,12 @@
     </row>
     <row r="49" spans="1:16">
       <c r="A49" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49" s="7" t="s"/>
       <c r="C49" s="6" t="s"/>
       <c r="D49" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E49" s="9">
         <f>E50+E52+E54</f>
@@ -2121,12 +2167,14 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s"/>
+      <c r="C50" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D50" s="3" t="s"/>
       <c r="E50" s="14">
         <f>E51</f>
@@ -2156,7 +2204,7 @@
     </row>
     <row hidden="1" r="51" spans="1:16">
       <c r="A51" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B51" s="16" t="n">
         <v>0</v>
@@ -2178,12 +2226,14 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s"/>
+      <c r="C52" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D52" s="3" t="s"/>
       <c r="E52" s="14">
         <f>E53</f>
@@ -2213,7 +2263,7 @@
     </row>
     <row hidden="1" r="53" spans="1:16">
       <c r="A53" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B53" s="16" t="n">
         <v>0</v>
@@ -2235,12 +2285,14 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C54" s="1" t="s"/>
+      <c r="C54" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D54" s="3" t="s"/>
       <c r="E54" s="14">
         <f>E55</f>
@@ -2270,7 +2322,7 @@
     </row>
     <row hidden="1" r="55" spans="1:16">
       <c r="A55" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B55" s="16" t="n">
         <v>0</v>
@@ -2292,12 +2344,12 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56" s="7" t="s"/>
       <c r="C56" s="6" t="s"/>
       <c r="D56" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E56" s="9">
         <f>E57</f>
@@ -2318,7 +2370,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="11" t="s"/>
       <c r="C57" s="10" t="s"/>
@@ -2342,7 +2394,7 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="19" t="s"/>
       <c r="C58" s="18" t="s"/>
@@ -2366,7 +2418,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="22" t="s"/>
       <c r="C59" s="21" t="s"/>
@@ -2390,7 +2442,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="25" t="s"/>
       <c r="C60" s="24" t="s"/>
@@ -2414,7 +2466,7 @@
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2" t="s"/>
       <c r="C61" s="1" t="s"/>
@@ -2438,7 +2490,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="2" t="s"/>
       <c r="C62" s="1" t="s"/>
@@ -2462,7 +2514,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63" s="2" t="s"/>
       <c r="C63" s="1" t="s"/>
@@ -2486,12 +2538,14 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C64" s="1" t="s"/>
+      <c r="C64" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D64" s="3" t="s"/>
       <c r="E64" s="14">
         <f>E65</f>
@@ -2521,7 +2575,7 @@
     </row>
     <row hidden="1" r="65" spans="1:16">
       <c r="A65" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" s="16" t="n">
         <v>0</v>
@@ -2543,12 +2597,14 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="s"/>
+      <c r="C66" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D66" s="3" t="s"/>
       <c r="E66" s="14">
         <f>E67</f>
@@ -2578,7 +2634,7 @@
     </row>
     <row hidden="1" r="67" spans="1:16">
       <c r="A67" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B67" s="16" t="n">
         <v>0</v>
@@ -2600,7 +2656,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B68" s="22" t="s"/>
       <c r="C68" s="21" t="s"/>
@@ -2624,7 +2680,7 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B69" s="25" t="s"/>
       <c r="C69" s="24" t="s"/>
@@ -2648,7 +2704,7 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B70" s="2" t="s"/>
       <c r="C70" s="1" t="s"/>
@@ -2672,12 +2728,14 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C71" s="1" t="s"/>
+      <c r="C71" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D71" s="3" t="s"/>
       <c r="E71" s="14">
         <f>E72</f>
@@ -2707,7 +2765,7 @@
     </row>
     <row hidden="1" r="72" spans="1:16">
       <c r="A72" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B72" s="16" t="n">
         <v>0</v>
@@ -2729,7 +2787,7 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B73" s="19" t="s"/>
       <c r="C73" s="18" t="s"/>
@@ -2753,7 +2811,7 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B74" s="22" t="s"/>
       <c r="C74" s="21" t="s"/>
@@ -2777,12 +2835,14 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C75" s="1" t="s"/>
+      <c r="C75" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D75" s="3" t="s"/>
       <c r="E75" s="14">
         <f>E76</f>
@@ -2812,7 +2872,7 @@
     </row>
     <row hidden="1" r="76" spans="1:16">
       <c r="A76" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B76" s="16" t="n">
         <v>0</v>
@@ -2834,7 +2894,7 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B78" s="27" t="s"/>
       <c r="C78" s="27" t="s"/>
@@ -2867,7 +2927,7 @@
     </row>
     <row r="79" spans="1:16">
       <c r="A79" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B79" s="27" t="s"/>
       <c r="C79" s="27" t="s"/>
@@ -2887,7 +2947,7 @@
     </row>
     <row r="80" spans="1:16">
       <c r="A80" s="27" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B80" s="27" t="s"/>
       <c r="C80" s="27" t="s"/>
@@ -2907,7 +2967,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="27" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B81" s="27" t="s"/>
       <c r="C81" s="27" t="s"/>
@@ -2927,7 +2987,7 @@
     </row>
     <row r="82" spans="1:16">
       <c r="A82" s="27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B82" s="27" t="s"/>
       <c r="C82" s="27" t="s"/>
@@ -2946,47 +3006,80 @@
       </c>
     </row>
     <row r="84" spans="1:16">
-      <c r="A84" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C84" s="14">
-        <f>SQRT(K78)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:16">
-      <c r="A85" s="29" t="s">
+      <c r="A84" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C85" s="14" t="n">
+      <c r="B84" s="27" t="s"/>
+      <c r="C84" s="27" t="s"/>
+      <c r="D84" s="27" t="s"/>
+      <c r="E84" s="28">
+        <f>SUMPRODUCT(E2:E77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+      <c r="F84" s="28">
+        <f>SUMPRODUCT(F2:F77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+      <c r="G84" s="28">
+        <f>SUMPRODUCT(G2:G77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+      <c r="H84" s="27" t="s"/>
+      <c r="I84" s="28">
+        <f>SUMPRODUCT(I2:I77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+      <c r="J84" s="28">
+        <f>SUMPRODUCT(J2:J77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+      <c r="K84" s="28">
+        <f>SUMPRODUCT(K2:K77,B2:B77,C2:C77)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
+      <c r="A86" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C86" s="14">
+        <f>SQRT(K84)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
+      <c r="A87" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="14" t="n">
         <v>1.5</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
-      <c r="A86" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B86" s="27" t="s"/>
-      <c r="C86" s="28">
-        <f>I78-2*C84</f>
-        <v/>
-      </c>
-      <c r="D86" s="30">
-        <f>C86*C85</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:16">
-      <c r="A87" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B87" s="27" t="s"/>
-      <c r="C87" s="28">
-        <f>I78+2*C84</f>
-        <v/>
-      </c>
-      <c r="D87" s="30">
-        <f>C87*C85</f>
+    <row r="88" spans="1:16">
+      <c r="A88" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" s="27" t="s"/>
+      <c r="C88" s="28">
+        <f>I84-2*C86</f>
+        <v/>
+      </c>
+      <c r="D88" s="30">
+        <f>C88*C87</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
+      <c r="A89" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" s="27" t="s"/>
+      <c r="C89" s="28">
+        <f>I84+2*C86</f>
+        <v/>
+      </c>
+      <c r="D89" s="30">
+        <f>C89*C87</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
MVP column, option, total row, data validation + option
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -720,7 +720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:Z87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,9 +743,10 @@
     <col customWidth="1" hidden="1" max="14" min="14" style="1" width="10"/>
     <col customWidth="1" hidden="1" max="15" min="15" style="1" width="10"/>
     <col customWidth="1" hidden="1" max="16" min="16" style="1" width="10"/>
+    <col hidden="1" max="26" min="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:26">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -787,8 +788,9 @@
       <c r="P1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Z1" s="2" t="s"/>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -813,8 +815,11 @@
       <c r="I2" s="6" t="s"/>
       <c r="J2" s="6" t="s"/>
       <c r="K2" s="6" t="s"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Z2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
@@ -837,8 +842,11 @@
       <c r="I3" s="10" t="s"/>
       <c r="J3" s="10" t="s"/>
       <c r="K3" s="10" t="s"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Z3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -873,7 +881,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="5" spans="1:16">
+    <row hidden="1" r="5" spans="1:26">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -895,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:26">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -930,7 +938,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="7" spans="1:16">
+    <row hidden="1" r="7" spans="1:26">
       <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
@@ -952,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:26">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -987,7 +995,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="9" spans="1:16">
+    <row hidden="1" r="9" spans="1:26">
       <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
@@ -1009,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:26">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1044,7 +1052,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="11" spans="1:16">
+    <row hidden="1" r="11" spans="1:26">
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:26">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -1090,7 +1098,7 @@
       <c r="J12" s="10" t="s"/>
       <c r="K12" s="10" t="s"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1125,7 +1133,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="14" spans="1:16">
+    <row hidden="1" r="14" spans="1:26">
       <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:26">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="16" spans="1:16">
+    <row hidden="1" r="16" spans="1:26">
       <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
@@ -1204,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:26">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +1247,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="18" spans="1:16">
+    <row hidden="1" r="18" spans="1:26">
       <c r="A18" s="15" t="s">
         <v>26</v>
       </c>
@@ -1261,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:26">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="20" spans="1:16">
+    <row hidden="1" r="20" spans="1:26">
       <c r="A20" s="15" t="s">
         <v>26</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:26">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -1344,7 +1352,7 @@
       <c r="J21" s="6" t="s"/>
       <c r="K21" s="6" t="s"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:26">
       <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1378,7 @@
       <c r="J22" s="10" t="s"/>
       <c r="K22" s="10" t="s"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:26">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1405,7 +1413,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="24" spans="1:16">
+    <row hidden="1" r="24" spans="1:26">
       <c r="A24" s="15" t="s">
         <v>17</v>
       </c>
@@ -1427,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:26">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1462,7 +1470,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="26" spans="1:16">
+    <row hidden="1" r="26" spans="1:26">
       <c r="A26" s="15" t="s">
         <v>17</v>
       </c>
@@ -1484,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:26">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="28" spans="1:16">
+    <row hidden="1" r="28" spans="1:26">
       <c r="A28" s="15" t="s">
         <v>17</v>
       </c>
@@ -1541,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:26">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1576,7 +1584,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="30" spans="1:16">
+    <row hidden="1" r="30" spans="1:26">
       <c r="A30" s="15" t="s">
         <v>26</v>
       </c>
@@ -1598,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row hidden="1" r="31" spans="1:16">
+    <row hidden="1" r="31" spans="1:26">
       <c r="A31" s="15" t="s">
         <v>36</v>
       </c>
@@ -1620,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:26">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1655,7 +1663,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="33" spans="1:16">
+    <row hidden="1" r="33" spans="1:26">
       <c r="A33" s="15" t="s">
         <v>26</v>
       </c>
@@ -1677,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row hidden="1" r="34" spans="1:16">
+    <row hidden="1" r="34" spans="1:26">
       <c r="A34" s="15" t="s">
         <v>36</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:26">
       <c r="A35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1725,7 +1733,7 @@
       <c r="J35" s="6" t="s"/>
       <c r="K35" s="6" t="s"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:26">
       <c r="A36" s="10" t="s">
         <v>40</v>
       </c>
@@ -1749,7 +1757,7 @@
       <c r="J36" s="10" t="s"/>
       <c r="K36" s="10" t="s"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:26">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1784,7 +1792,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="38" spans="1:16">
+    <row hidden="1" r="38" spans="1:26">
       <c r="A38" s="15" t="s">
         <v>23</v>
       </c>
@@ -1806,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:26">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1841,7 +1849,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="40" spans="1:16">
+    <row hidden="1" r="40" spans="1:26">
       <c r="A40" s="15" t="s">
         <v>23</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:26">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1898,7 +1906,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="42" spans="1:16">
+    <row hidden="1" r="42" spans="1:26">
       <c r="A42" s="15" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:26">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1955,7 +1963,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="44" spans="1:16">
+    <row hidden="1" r="44" spans="1:26">
       <c r="A44" s="15" t="s">
         <v>26</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:26">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2012,7 +2020,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="46" spans="1:16">
+    <row hidden="1" r="46" spans="1:26">
       <c r="A46" s="15" t="s">
         <v>26</v>
       </c>
@@ -2034,7 +2042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:26">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -2071,7 +2079,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="48" spans="1:16">
+    <row hidden="1" r="48" spans="1:26">
       <c r="A48" s="15" t="s">
         <v>26</v>
       </c>
@@ -2093,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:26">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -2119,7 +2127,7 @@
       <c r="J49" s="6" t="s"/>
       <c r="K49" s="6" t="s"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:26">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2154,7 +2162,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="51" spans="1:16">
+    <row hidden="1" r="51" spans="1:26">
       <c r="A51" s="15" t="s">
         <v>26</v>
       </c>
@@ -2176,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:26">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -2211,7 +2219,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="53" spans="1:16">
+    <row hidden="1" r="53" spans="1:26">
       <c r="A53" s="15" t="s">
         <v>26</v>
       </c>
@@ -2233,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:26">
       <c r="A54" s="1" t="s">
         <v>37</v>
       </c>
@@ -2268,7 +2276,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="55" spans="1:16">
+    <row hidden="1" r="55" spans="1:26">
       <c r="A55" s="15" t="s">
         <v>36</v>
       </c>
@@ -2290,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:26">
       <c r="A56" s="6" t="s">
         <v>53</v>
       </c>
@@ -2316,7 +2324,7 @@
       <c r="J56" s="6" t="s"/>
       <c r="K56" s="6" t="s"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:26">
       <c r="A57" s="10" t="s">
         <v>55</v>
       </c>
@@ -2340,7 +2348,7 @@
       <c r="J57" s="10" t="s"/>
       <c r="K57" s="10" t="s"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:26">
       <c r="A58" s="18" t="s">
         <v>56</v>
       </c>
@@ -2364,7 +2372,7 @@
       <c r="J58" s="18" t="s"/>
       <c r="K58" s="18" t="s"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:26">
       <c r="A59" s="21" t="s">
         <v>57</v>
       </c>
@@ -2388,7 +2396,7 @@
       <c r="J59" s="21" t="s"/>
       <c r="K59" s="21" t="s"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:26">
       <c r="A60" s="24" t="s">
         <v>58</v>
       </c>
@@ -2412,7 +2420,7 @@
       <c r="J60" s="24" t="s"/>
       <c r="K60" s="24" t="s"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:26">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -2436,7 +2444,7 @@
       <c r="J61" s="1" t="s"/>
       <c r="K61" s="1" t="s"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:26">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -2460,7 +2468,7 @@
       <c r="J62" s="1" t="s"/>
       <c r="K62" s="1" t="s"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:26">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -2484,7 +2492,7 @@
       <c r="J63" s="1" t="s"/>
       <c r="K63" s="1" t="s"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:26">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -2519,7 +2527,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="65" spans="1:16">
+    <row hidden="1" r="65" spans="1:26">
       <c r="A65" s="15" t="s">
         <v>63</v>
       </c>
@@ -2541,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:26">
       <c r="A66" s="1" t="s">
         <v>60</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="67" spans="1:16">
+    <row hidden="1" r="67" spans="1:26">
       <c r="A67" s="15" t="s">
         <v>64</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:26">
       <c r="A68" s="21" t="s">
         <v>57</v>
       </c>
@@ -2622,7 +2630,7 @@
       <c r="J68" s="21" t="s"/>
       <c r="K68" s="21" t="s"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:26">
       <c r="A69" s="24" t="s">
         <v>58</v>
       </c>
@@ -2646,7 +2654,7 @@
       <c r="J69" s="24" t="s"/>
       <c r="K69" s="24" t="s"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:26">
       <c r="A70" s="1" t="s">
         <v>59</v>
       </c>
@@ -2670,7 +2678,7 @@
       <c r="J70" s="1" t="s"/>
       <c r="K70" s="1" t="s"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:26">
       <c r="A71" s="1" t="s">
         <v>60</v>
       </c>
@@ -2705,7 +2713,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="72" spans="1:16">
+    <row hidden="1" r="72" spans="1:26">
       <c r="A72" s="15" t="s">
         <v>64</v>
       </c>
@@ -2727,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:26">
       <c r="A73" s="18" t="s">
         <v>56</v>
       </c>
@@ -2751,7 +2759,7 @@
       <c r="J73" s="18" t="s"/>
       <c r="K73" s="18" t="s"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:26">
       <c r="A74" s="21" t="s">
         <v>57</v>
       </c>
@@ -2775,7 +2783,7 @@
       <c r="J74" s="21" t="s"/>
       <c r="K74" s="21" t="s"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:26">
       <c r="A75" s="1" t="s">
         <v>58</v>
       </c>
@@ -2810,7 +2818,7 @@
         <v/>
       </c>
     </row>
-    <row hidden="1" r="76" spans="1:16">
+    <row hidden="1" r="76" spans="1:26">
       <c r="A76" s="15" t="s">
         <v>65</v>
       </c>
@@ -2832,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:26">
       <c r="A78" s="27" t="s">
         <v>66</v>
       </c>
@@ -2865,7 +2873,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:26">
       <c r="A79" s="27" t="s">
         <v>67</v>
       </c>
@@ -2885,7 +2893,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:26">
       <c r="A80" s="27" t="s">
         <v>68</v>
       </c>
@@ -2905,7 +2913,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:26">
       <c r="A81" s="27" t="s">
         <v>69</v>
       </c>
@@ -2925,7 +2933,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:26">
       <c r="A82" s="27" t="s">
         <v>70</v>
       </c>
@@ -2945,7 +2953,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:26">
       <c r="A84" s="29" t="s">
         <v>71</v>
       </c>
@@ -2954,7 +2962,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:26">
       <c r="A85" s="29" t="s">
         <v>72</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:26">
       <c r="A86" s="27" t="s">
         <v>73</v>
       </c>
@@ -2976,7 +2984,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:26">
       <c r="A87" s="27" t="s">
         <v>74</v>
       </c>
@@ -2992,6 +3000,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K77"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showDropDown="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B77" type="list">
+      <formula1>$Z$1:$Z$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Role & Stage columns filters by column, global factor (fix tests)
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>Task / Subtask</t>
   </si>
@@ -48,16 +48,7 @@
     <t>Sq</t>
   </si>
   <si>
-    <t>(adm)</t>
-  </si>
-  <si>
-    <t>(analysis)</t>
-  </si>
-  <si>
-    <t>(coding)</t>
-  </si>
-  <si>
-    <t>(test)</t>
+    <t>Role</t>
   </si>
   <si>
     <t>Stage 1: Implement the Idea</t>
@@ -237,7 +228,7 @@
     <t>Standard deviation</t>
   </si>
   <si>
-    <t>O</t>
+    <t>K</t>
   </si>
   <si>
     <t>Min (P=95%)</t>
@@ -749,10 +740,7 @@
     <col customWidth="1" max="13" min="13" style="4" width="8"/>
     <col customWidth="1" max="14" min="14" style="4" width="8"/>
     <col customWidth="1" max="15" min="15" style="4" width="8"/>
-    <col customWidth="1" hidden="1" max="27" min="27" style="1" width="10"/>
-    <col customWidth="1" hidden="1" max="28" min="28" style="1" width="10"/>
-    <col customWidth="1" hidden="1" max="29" min="29" style="1" width="10"/>
-    <col customWidth="1" hidden="1" max="30" min="30" style="1" width="10"/>
+    <col customWidth="1" hidden="1" max="16" min="16" style="1" width="3"/>
     <col hidden="1" max="52" min="52"/>
   </cols>
   <sheetData>
@@ -792,23 +780,14 @@
       <c r="O1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="AZ1" s="2" t="s"/>
     </row>
     <row r="2" spans="1:52">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="7" t="s"/>
       <c r="C2" s="6" t="s"/>
@@ -817,7 +796,7 @@
       <c r="F2" s="6" t="s"/>
       <c r="G2" s="6" t="s"/>
       <c r="H2" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2" s="9">
         <f>I3+I12+I17+I19</f>
@@ -835,13 +814,14 @@
       <c r="M2" s="6" t="s"/>
       <c r="N2" s="6" t="s"/>
       <c r="O2" s="6" t="s"/>
+      <c r="P2" s="6" t="s"/>
       <c r="AZ2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="11" t="s"/>
       <c r="C3" s="10" t="s"/>
@@ -866,13 +846,14 @@
       <c r="M3" s="10" t="s"/>
       <c r="N3" s="10" t="s"/>
       <c r="O3" s="10" t="s"/>
+      <c r="P3" s="10" t="s"/>
       <c r="AZ3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -908,10 +889,11 @@
         <f>N4*N4</f>
         <v/>
       </c>
+      <c r="P4" s="1" t="s"/>
     </row>
     <row hidden="1" r="5" spans="1:52">
       <c r="A5" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="16" t="n">
         <v>0</v>
@@ -931,13 +913,14 @@
       <c r="K5" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB5" s="4" t="n">
-        <v>1</v>
+      <c r="P5" s="4">
+        <f>TRIM(A5)</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:52">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
@@ -973,10 +956,11 @@
         <f>N6*N6</f>
         <v/>
       </c>
+      <c r="P6" s="1" t="s"/>
     </row>
     <row hidden="1" r="7" spans="1:52">
       <c r="A7" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="16" t="n">
         <v>0</v>
@@ -996,13 +980,14 @@
       <c r="K7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="AB7" s="4" t="n">
-        <v>1</v>
+      <c r="P7" s="4">
+        <f>TRIM(A7)</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:52">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
@@ -1038,10 +1023,11 @@
         <f>N8*N8</f>
         <v/>
       </c>
+      <c r="P8" s="1" t="s"/>
     </row>
     <row hidden="1" r="9" spans="1:52">
       <c r="A9" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="16" t="n">
         <v>0</v>
@@ -1061,13 +1047,14 @@
       <c r="K9" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="AB9" s="4" t="n">
-        <v>1</v>
+      <c r="P9" s="4">
+        <f>TRIM(A9)</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:52">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
@@ -1103,10 +1090,11 @@
         <f>N10*N10</f>
         <v/>
       </c>
+      <c r="P10" s="1" t="s"/>
     </row>
     <row hidden="1" r="11" spans="1:52">
       <c r="A11" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="16" t="n">
         <v>0</v>
@@ -1126,13 +1114,14 @@
       <c r="K11" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="AB11" s="4" t="n">
-        <v>1</v>
+      <c r="P11" s="4">
+        <f>TRIM(A11)</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:52">
       <c r="A12" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11" t="s"/>
       <c r="C12" s="10" t="s"/>
@@ -1157,10 +1146,11 @@
       <c r="M12" s="10" t="s"/>
       <c r="N12" s="10" t="s"/>
       <c r="O12" s="10" t="s"/>
+      <c r="P12" s="10" t="s"/>
     </row>
     <row r="13" spans="1:52">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
@@ -1196,10 +1186,11 @@
         <f>N13*N13</f>
         <v/>
       </c>
+      <c r="P13" s="1" t="s"/>
     </row>
     <row hidden="1" r="14" spans="1:52">
       <c r="A14" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="16" t="n">
         <v>0</v>
@@ -1219,13 +1210,14 @@
       <c r="K14" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AC14" s="4" t="n">
-        <v>1</v>
+      <c r="P14" s="4">
+        <f>TRIM(A14)</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:52">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
@@ -1261,10 +1253,11 @@
         <f>N15*N15</f>
         <v/>
       </c>
+      <c r="P15" s="1" t="s"/>
     </row>
     <row hidden="1" r="16" spans="1:52">
       <c r="A16" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="16" t="n">
         <v>0</v>
@@ -1284,13 +1277,14 @@
       <c r="K16" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AC16" s="4" t="n">
-        <v>1</v>
+      <c r="P16" s="4">
+        <f>TRIM(A16)</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:52">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
@@ -1326,10 +1320,11 @@
         <f>N17*N17</f>
         <v/>
       </c>
+      <c r="P17" s="1" t="s"/>
     </row>
     <row hidden="1" r="18" spans="1:52">
       <c r="A18" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="16" t="n">
         <v>0</v>
@@ -1349,13 +1344,14 @@
       <c r="K18" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AB18" s="4" t="n">
-        <v>1</v>
+      <c r="P18" s="4">
+        <f>TRIM(A18)</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:52">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>1</v>
@@ -1391,10 +1387,11 @@
         <f>N19*N19</f>
         <v/>
       </c>
+      <c r="P19" s="1" t="s"/>
     </row>
     <row hidden="1" r="20" spans="1:52">
       <c r="A20" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="16" t="n">
         <v>0</v>
@@ -1414,13 +1411,14 @@
       <c r="K20" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB20" s="4" t="n">
-        <v>1</v>
+      <c r="P20" s="4">
+        <f>TRIM(A20)</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:52">
       <c r="A21" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" s="7" t="s"/>
       <c r="C21" s="6" t="s"/>
@@ -1429,7 +1427,7 @@
       <c r="F21" s="6" t="s"/>
       <c r="G21" s="6" t="s"/>
       <c r="H21" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I21" s="9">
         <f>I22+I29+I32</f>
@@ -1447,10 +1445,11 @@
       <c r="M21" s="6" t="s"/>
       <c r="N21" s="6" t="s"/>
       <c r="O21" s="6" t="s"/>
+      <c r="P21" s="6" t="s"/>
     </row>
     <row r="22" spans="1:52">
       <c r="A22" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" s="11" t="s"/>
       <c r="C22" s="10" t="s"/>
@@ -1459,7 +1458,7 @@
       <c r="F22" s="10" t="s"/>
       <c r="G22" s="10" t="s"/>
       <c r="H22" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I22" s="13">
         <f>I23+I25+I27</f>
@@ -1477,10 +1476,11 @@
       <c r="M22" s="10" t="s"/>
       <c r="N22" s="10" t="s"/>
       <c r="O22" s="10" t="s"/>
+      <c r="P22" s="10" t="s"/>
     </row>
     <row r="23" spans="1:52">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>1</v>
@@ -1516,10 +1516,11 @@
         <f>N23*N23</f>
         <v/>
       </c>
+      <c r="P23" s="1" t="s"/>
     </row>
     <row hidden="1" r="24" spans="1:52">
       <c r="A24" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B24" s="16" t="n">
         <v>0</v>
@@ -1539,13 +1540,14 @@
       <c r="K24" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="AB24" s="4" t="n">
-        <v>1</v>
+      <c r="P24" s="4">
+        <f>TRIM(A24)</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:52">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>1</v>
@@ -1581,10 +1583,11 @@
         <f>N25*N25</f>
         <v/>
       </c>
+      <c r="P25" s="1" t="s"/>
     </row>
     <row hidden="1" r="26" spans="1:52">
       <c r="A26" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B26" s="16" t="n">
         <v>0</v>
@@ -1604,13 +1607,14 @@
       <c r="K26" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="AB26" s="4" t="n">
-        <v>1</v>
+      <c r="P26" s="4">
+        <f>TRIM(A26)</f>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:52">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>1</v>
@@ -1646,10 +1650,11 @@
         <f>N27*N27</f>
         <v/>
       </c>
+      <c r="P27" s="1" t="s"/>
     </row>
     <row hidden="1" r="28" spans="1:52">
       <c r="A28" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B28" s="16" t="n">
         <v>0</v>
@@ -1669,13 +1674,14 @@
       <c r="K28" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB28" s="4" t="n">
-        <v>1</v>
+      <c r="P28" s="4">
+        <f>TRIM(A28)</f>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:52">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>1</v>
@@ -1711,10 +1717,11 @@
         <f>N29*N29</f>
         <v/>
       </c>
+      <c r="P29" s="1" t="s"/>
     </row>
     <row hidden="1" r="30" spans="1:52">
       <c r="A30" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="16" t="n">
         <v>0</v>
@@ -1734,13 +1741,14 @@
       <c r="K30" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB30" s="4" t="n">
-        <v>1</v>
+      <c r="P30" s="4">
+        <f>TRIM(A30)</f>
+        <v/>
       </c>
     </row>
     <row hidden="1" r="31" spans="1:52">
       <c r="A31" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31" s="16" t="n">
         <v>0</v>
@@ -1760,13 +1768,14 @@
       <c r="K31" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="AC31" s="4" t="n">
-        <v>1</v>
+      <c r="P31" s="4">
+        <f>TRIM(A31)</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:52">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1</v>
@@ -1802,10 +1811,11 @@
         <f>N32*N32</f>
         <v/>
       </c>
+      <c r="P32" s="1" t="s"/>
     </row>
     <row hidden="1" r="33" spans="1:52">
       <c r="A33" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B33" s="16" t="n">
         <v>0</v>
@@ -1825,13 +1835,14 @@
       <c r="K33" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB33" s="4" t="n">
-        <v>1</v>
+      <c r="P33" s="4">
+        <f>TRIM(A33)</f>
+        <v/>
       </c>
     </row>
     <row hidden="1" r="34" spans="1:52">
       <c r="A34" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="16" t="n">
         <v>0</v>
@@ -1851,13 +1862,14 @@
       <c r="K34" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AC34" s="4" t="n">
-        <v>1</v>
+      <c r="P34" s="4">
+        <f>TRIM(A34)</f>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:52">
       <c r="A35" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B35" s="7" t="s"/>
       <c r="C35" s="6" t="s"/>
@@ -1866,7 +1878,7 @@
       <c r="F35" s="6" t="s"/>
       <c r="G35" s="6" t="s"/>
       <c r="H35" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I35" s="9">
         <f>I36+I41+I43+I45+I47</f>
@@ -1884,10 +1896,11 @@
       <c r="M35" s="6" t="s"/>
       <c r="N35" s="6" t="s"/>
       <c r="O35" s="6" t="s"/>
+      <c r="P35" s="6" t="s"/>
     </row>
     <row r="36" spans="1:52">
       <c r="A36" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="11" t="s"/>
       <c r="C36" s="10" t="s"/>
@@ -1912,10 +1925,11 @@
       <c r="M36" s="10" t="s"/>
       <c r="N36" s="10" t="s"/>
       <c r="O36" s="10" t="s"/>
+      <c r="P36" s="10" t="s"/>
     </row>
     <row r="37" spans="1:52">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1</v>
@@ -1951,10 +1965,11 @@
         <f>N37*N37</f>
         <v/>
       </c>
+      <c r="P37" s="1" t="s"/>
     </row>
     <row hidden="1" r="38" spans="1:52">
       <c r="A38" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B38" s="16" t="n">
         <v>0</v>
@@ -1974,13 +1989,14 @@
       <c r="K38" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AC38" s="4" t="n">
-        <v>1</v>
+      <c r="P38" s="4">
+        <f>TRIM(A38)</f>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:52">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>1</v>
@@ -2016,10 +2032,11 @@
         <f>N39*N39</f>
         <v/>
       </c>
+      <c r="P39" s="1" t="s"/>
     </row>
     <row hidden="1" r="40" spans="1:52">
       <c r="A40" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B40" s="16" t="n">
         <v>0</v>
@@ -2039,13 +2056,14 @@
       <c r="K40" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AC40" s="4" t="n">
-        <v>1</v>
+      <c r="P40" s="4">
+        <f>TRIM(A40)</f>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:52">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>1</v>
@@ -2081,10 +2099,11 @@
         <f>N41*N41</f>
         <v/>
       </c>
+      <c r="P41" s="1" t="s"/>
     </row>
     <row hidden="1" r="42" spans="1:52">
       <c r="A42" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B42" s="16" t="n">
         <v>0</v>
@@ -2104,13 +2123,14 @@
       <c r="K42" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AA42" s="4" t="n">
-        <v>1</v>
+      <c r="P42" s="4">
+        <f>TRIM(A42)</f>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:52">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>1</v>
@@ -2146,10 +2166,11 @@
         <f>N43*N43</f>
         <v/>
       </c>
+      <c r="P43" s="1" t="s"/>
     </row>
     <row hidden="1" r="44" spans="1:52">
       <c r="A44" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B44" s="16" t="n">
         <v>0</v>
@@ -2169,13 +2190,14 @@
       <c r="K44" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AB44" s="4" t="n">
-        <v>1</v>
+      <c r="P44" s="4">
+        <f>TRIM(A44)</f>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:52">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1</v>
@@ -2211,10 +2233,11 @@
         <f>N45*N45</f>
         <v/>
       </c>
+      <c r="P45" s="1" t="s"/>
     </row>
     <row hidden="1" r="46" spans="1:52">
       <c r="A46" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B46" s="16" t="n">
         <v>0</v>
@@ -2234,13 +2257,14 @@
       <c r="K46" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB46" s="4" t="n">
-        <v>1</v>
+      <c r="P46" s="4">
+        <f>TRIM(A46)</f>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:52">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>1</v>
@@ -2251,7 +2275,7 @@
       <c r="F47" s="1" t="s"/>
       <c r="G47" s="1" t="s"/>
       <c r="H47" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I47" s="14">
         <f>I48</f>
@@ -2278,10 +2302,11 @@
         <f>N47*N47</f>
         <v/>
       </c>
+      <c r="P47" s="1" t="s"/>
     </row>
     <row hidden="1" r="48" spans="1:52">
       <c r="A48" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B48" s="16" t="n">
         <v>0</v>
@@ -2301,13 +2326,14 @@
       <c r="K48" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="AB48" s="4" t="n">
-        <v>1</v>
+      <c r="P48" s="4">
+        <f>TRIM(A48)</f>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:52">
       <c r="A49" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7" t="s"/>
       <c r="C49" s="6" t="s"/>
@@ -2316,7 +2342,7 @@
       <c r="F49" s="6" t="s"/>
       <c r="G49" s="6" t="s"/>
       <c r="H49" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I49" s="9">
         <f>I50+I52+I54</f>
@@ -2334,10 +2360,11 @@
       <c r="M49" s="6" t="s"/>
       <c r="N49" s="6" t="s"/>
       <c r="O49" s="6" t="s"/>
+      <c r="P49" s="6" t="s"/>
     </row>
     <row r="50" spans="1:52">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>1</v>
@@ -2373,10 +2400,11 @@
         <f>N50*N50</f>
         <v/>
       </c>
+      <c r="P50" s="1" t="s"/>
     </row>
     <row hidden="1" r="51" spans="1:52">
       <c r="A51" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B51" s="16" t="n">
         <v>0</v>
@@ -2396,13 +2424,14 @@
       <c r="K51" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="AB51" s="4" t="n">
-        <v>1</v>
+      <c r="P51" s="4">
+        <f>TRIM(A51)</f>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:52">
       <c r="A52" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>1</v>
@@ -2438,10 +2467,11 @@
         <f>N52*N52</f>
         <v/>
       </c>
+      <c r="P52" s="1" t="s"/>
     </row>
     <row hidden="1" r="53" spans="1:52">
       <c r="A53" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B53" s="16" t="n">
         <v>0</v>
@@ -2461,13 +2491,14 @@
       <c r="K53" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="AB53" s="4" t="n">
-        <v>1</v>
+      <c r="P53" s="4">
+        <f>TRIM(A53)</f>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:52">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>1</v>
@@ -2503,10 +2534,11 @@
         <f>N54*N54</f>
         <v/>
       </c>
+      <c r="P54" s="1" t="s"/>
     </row>
     <row hidden="1" r="55" spans="1:52">
       <c r="A55" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B55" s="16" t="n">
         <v>0</v>
@@ -2526,13 +2558,14 @@
       <c r="K55" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="AC55" s="4" t="n">
-        <v>1</v>
+      <c r="P55" s="4">
+        <f>TRIM(A55)</f>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:52">
       <c r="A56" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B56" s="7" t="s"/>
       <c r="C56" s="6" t="s"/>
@@ -2541,7 +2574,7 @@
       <c r="F56" s="6" t="s"/>
       <c r="G56" s="6" t="s"/>
       <c r="H56" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I56" s="9">
         <f>I57</f>
@@ -2559,10 +2592,11 @@
       <c r="M56" s="6" t="s"/>
       <c r="N56" s="6" t="s"/>
       <c r="O56" s="6" t="s"/>
+      <c r="P56" s="6" t="s"/>
     </row>
     <row r="57" spans="1:52">
       <c r="A57" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B57" s="11" t="s"/>
       <c r="C57" s="10" t="s"/>
@@ -2587,10 +2621,11 @@
       <c r="M57" s="10" t="s"/>
       <c r="N57" s="10" t="s"/>
       <c r="O57" s="10" t="s"/>
+      <c r="P57" s="10" t="s"/>
     </row>
     <row r="58" spans="1:52">
       <c r="A58" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B58" s="19" t="s"/>
       <c r="C58" s="18" t="s"/>
@@ -2615,10 +2650,11 @@
       <c r="M58" s="18" t="s"/>
       <c r="N58" s="18" t="s"/>
       <c r="O58" s="18" t="s"/>
+      <c r="P58" s="18" t="s"/>
     </row>
     <row r="59" spans="1:52">
       <c r="A59" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B59" s="22" t="s"/>
       <c r="C59" s="21" t="s"/>
@@ -2643,10 +2679,11 @@
       <c r="M59" s="21" t="s"/>
       <c r="N59" s="21" t="s"/>
       <c r="O59" s="21" t="s"/>
+      <c r="P59" s="21" t="s"/>
     </row>
     <row r="60" spans="1:52">
       <c r="A60" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B60" s="25" t="s"/>
       <c r="C60" s="24" t="s"/>
@@ -2671,10 +2708,11 @@
       <c r="M60" s="24" t="s"/>
       <c r="N60" s="24" t="s"/>
       <c r="O60" s="24" t="s"/>
+      <c r="P60" s="24" t="s"/>
     </row>
     <row r="61" spans="1:52">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61" s="2" t="s"/>
       <c r="C61" s="1" t="s"/>
@@ -2699,10 +2737,11 @@
       <c r="M61" s="1" t="s"/>
       <c r="N61" s="1" t="s"/>
       <c r="O61" s="1" t="s"/>
+      <c r="P61" s="1" t="s"/>
     </row>
     <row r="62" spans="1:52">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62" s="2" t="s"/>
       <c r="C62" s="1" t="s"/>
@@ -2727,10 +2766,11 @@
       <c r="M62" s="1" t="s"/>
       <c r="N62" s="1" t="s"/>
       <c r="O62" s="1" t="s"/>
+      <c r="P62" s="1" t="s"/>
     </row>
     <row r="63" spans="1:52">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2" t="s"/>
       <c r="C63" s="1" t="s"/>
@@ -2755,10 +2795,11 @@
       <c r="M63" s="1" t="s"/>
       <c r="N63" s="1" t="s"/>
       <c r="O63" s="1" t="s"/>
+      <c r="P63" s="1" t="s"/>
     </row>
     <row r="64" spans="1:52">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>1</v>
@@ -2794,10 +2835,11 @@
         <f>N64*N64</f>
         <v/>
       </c>
+      <c r="P64" s="1" t="s"/>
     </row>
     <row hidden="1" r="65" spans="1:52">
       <c r="A65" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B65" s="16" t="n">
         <v>0</v>
@@ -2817,13 +2859,14 @@
       <c r="K65" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="AD65" s="4" t="n">
-        <v>1</v>
+      <c r="P65" s="4">
+        <f>TRIM(A65)</f>
+        <v/>
       </c>
     </row>
     <row r="66" spans="1:52">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>1</v>
@@ -2859,10 +2902,11 @@
         <f>N66*N66</f>
         <v/>
       </c>
+      <c r="P66" s="1" t="s"/>
     </row>
     <row hidden="1" r="67" spans="1:52">
       <c r="A67" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B67" s="16" t="n">
         <v>0</v>
@@ -2882,13 +2926,14 @@
       <c r="K67" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="AD67" s="4" t="n">
-        <v>1</v>
+      <c r="P67" s="4">
+        <f>TRIM(A67)</f>
+        <v/>
       </c>
     </row>
     <row r="68" spans="1:52">
       <c r="A68" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B68" s="22" t="s"/>
       <c r="C68" s="21" t="s"/>
@@ -2913,10 +2958,11 @@
       <c r="M68" s="21" t="s"/>
       <c r="N68" s="21" t="s"/>
       <c r="O68" s="21" t="s"/>
+      <c r="P68" s="21" t="s"/>
     </row>
     <row r="69" spans="1:52">
       <c r="A69" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B69" s="25" t="s"/>
       <c r="C69" s="24" t="s"/>
@@ -2941,10 +2987,11 @@
       <c r="M69" s="24" t="s"/>
       <c r="N69" s="24" t="s"/>
       <c r="O69" s="24" t="s"/>
+      <c r="P69" s="24" t="s"/>
     </row>
     <row r="70" spans="1:52">
       <c r="A70" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B70" s="2" t="s"/>
       <c r="C70" s="1" t="s"/>
@@ -2969,10 +3016,11 @@
       <c r="M70" s="1" t="s"/>
       <c r="N70" s="1" t="s"/>
       <c r="O70" s="1" t="s"/>
+      <c r="P70" s="1" t="s"/>
     </row>
     <row r="71" spans="1:52">
       <c r="A71" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>1</v>
@@ -3008,10 +3056,11 @@
         <f>N71*N71</f>
         <v/>
       </c>
+      <c r="P71" s="1" t="s"/>
     </row>
     <row hidden="1" r="72" spans="1:52">
       <c r="A72" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B72" s="16" t="n">
         <v>0</v>
@@ -3031,13 +3080,14 @@
       <c r="K72" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="AD72" s="4" t="n">
-        <v>1</v>
+      <c r="P72" s="4">
+        <f>TRIM(A72)</f>
+        <v/>
       </c>
     </row>
     <row r="73" spans="1:52">
       <c r="A73" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B73" s="19" t="s"/>
       <c r="C73" s="18" t="s"/>
@@ -3062,10 +3112,11 @@
       <c r="M73" s="18" t="s"/>
       <c r="N73" s="18" t="s"/>
       <c r="O73" s="18" t="s"/>
+      <c r="P73" s="18" t="s"/>
     </row>
     <row r="74" spans="1:52">
       <c r="A74" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B74" s="22" t="s"/>
       <c r="C74" s="21" t="s"/>
@@ -3090,10 +3141,11 @@
       <c r="M74" s="21" t="s"/>
       <c r="N74" s="21" t="s"/>
       <c r="O74" s="21" t="s"/>
+      <c r="P74" s="21" t="s"/>
     </row>
     <row r="75" spans="1:52">
       <c r="A75" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>1</v>
@@ -3129,10 +3181,11 @@
         <f>N75*N75</f>
         <v/>
       </c>
+      <c r="P75" s="1" t="s"/>
     </row>
     <row hidden="1" r="76" spans="1:52">
       <c r="A76" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B76" s="16" t="n">
         <v>0</v>
@@ -3152,13 +3205,14 @@
       <c r="K76" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="AD76" s="4" t="n">
-        <v>1</v>
+      <c r="P76" s="4">
+        <f>TRIM(A76)</f>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:52">
       <c r="A78" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B78" s="27" t="s"/>
       <c r="C78" s="27" t="s"/>
@@ -3168,34 +3222,34 @@
       <c r="G78" s="27" t="s"/>
       <c r="H78" s="27" t="s"/>
       <c r="I78" s="28">
-        <f>SUMPRODUCT(I2:I77,B2:B77)</f>
+        <f>SUMIFS(I2:I77,B2:B77,"=1")</f>
         <v/>
       </c>
       <c r="J78" s="28">
-        <f>SUMPRODUCT(J2:J77,B2:B77)</f>
+        <f>SUMIFS(J2:J77,B2:B77,"=1")</f>
         <v/>
       </c>
       <c r="K78" s="28">
-        <f>SUMPRODUCT(K2:K77,B2:B77)</f>
+        <f>SUMIFS(K2:K77,B2:B77,"=1")</f>
         <v/>
       </c>
       <c r="L78" s="27" t="s"/>
       <c r="M78" s="28">
-        <f>SUMPRODUCT(M2:M77,B2:B77)</f>
+        <f>SUMIFS(M2:M77,B2:B77,"=1")</f>
         <v/>
       </c>
       <c r="N78" s="28">
-        <f>SUMPRODUCT(N2:N77,B2:B77)</f>
+        <f>SUMIFS(N2:N77,B2:B77,"=1")</f>
         <v/>
       </c>
       <c r="O78" s="28">
-        <f>SUMPRODUCT(O2:O77,B2:B77)</f>
+        <f>SUMIFS(O2:O77,B2:B77,"=1")</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:52">
       <c r="A79" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B79" s="27" t="s"/>
       <c r="C79" s="27" t="s"/>
@@ -3205,15 +3259,15 @@
       <c r="G79" s="27" t="s"/>
       <c r="H79" s="27" t="s"/>
       <c r="I79" s="28">
-        <f>SUMPRODUCT(I2:I77,AA2:AA77)</f>
+        <f>SUMIFS(I2:I77,B2:B77,"=0",P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="J79" s="28">
-        <f>SUMPRODUCT(J2:J77,AA2:AA77)</f>
+        <f>SUMIFS(J2:J77,B2:B77,"=0",P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="K79" s="28">
-        <f>SUMPRODUCT(K2:K77,AA2:AA77)</f>
+        <f>SUMIFS(K2:K77,B2:B77,"=0",P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="M79" s="28">
@@ -3227,7 +3281,7 @@
     </row>
     <row r="80" spans="1:52">
       <c r="A80" s="27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B80" s="27" t="s"/>
       <c r="C80" s="27" t="s"/>
@@ -3237,15 +3291,15 @@
       <c r="G80" s="27" t="s"/>
       <c r="H80" s="27" t="s"/>
       <c r="I80" s="28">
-        <f>SUMPRODUCT(I2:I77,AB2:AB77)</f>
+        <f>SUMIFS(I2:I77,B2:B77,"=0",P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="J80" s="28">
-        <f>SUMPRODUCT(J2:J77,AB2:AB77)</f>
+        <f>SUMIFS(J2:J77,B2:B77,"=0",P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="K80" s="28">
-        <f>SUMPRODUCT(K2:K77,AB2:AB77)</f>
+        <f>SUMIFS(K2:K77,B2:B77,"=0",P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="M80" s="28">
@@ -3259,7 +3313,7 @@
     </row>
     <row r="81" spans="1:52">
       <c r="A81" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B81" s="27" t="s"/>
       <c r="C81" s="27" t="s"/>
@@ -3269,15 +3323,15 @@
       <c r="G81" s="27" t="s"/>
       <c r="H81" s="27" t="s"/>
       <c r="I81" s="28">
-        <f>SUMPRODUCT(I2:I77,AC2:AC77)</f>
+        <f>SUMIFS(I2:I77,B2:B77,"=0",P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="J81" s="28">
-        <f>SUMPRODUCT(J2:J77,AC2:AC77)</f>
+        <f>SUMIFS(J2:J77,B2:B77,"=0",P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="K81" s="28">
-        <f>SUMPRODUCT(K2:K77,AC2:AC77)</f>
+        <f>SUMIFS(K2:K77,B2:B77,"=0",P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="M81" s="28">
@@ -3291,7 +3345,7 @@
     </row>
     <row r="82" spans="1:52">
       <c r="A82" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B82" s="27" t="s"/>
       <c r="C82" s="27" t="s"/>
@@ -3301,15 +3355,15 @@
       <c r="G82" s="27" t="s"/>
       <c r="H82" s="27" t="s"/>
       <c r="I82" s="28">
-        <f>SUMPRODUCT(I2:I77,AD2:AD77)</f>
+        <f>SUMIFS(I2:I77,B2:B77,"=0",P2:P77,"(test)")</f>
         <v/>
       </c>
       <c r="J82" s="28">
-        <f>SUMPRODUCT(J2:J77,AD2:AD77)</f>
+        <f>SUMIFS(J2:J77,B2:B77,"=0",P2:P77,"(test)")</f>
         <v/>
       </c>
       <c r="K82" s="28">
-        <f>SUMPRODUCT(K2:K77,AD2:AD77)</f>
+        <f>SUMIFS(K2:K77,B2:B77,"=0",P2:P77,"(test)")</f>
         <v/>
       </c>
       <c r="M82" s="28">
@@ -3323,7 +3377,7 @@
     </row>
     <row r="84" spans="1:52">
       <c r="A84" s="30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C84" s="14">
         <f>SQRT(O78)</f>
@@ -3332,7 +3386,7 @@
     </row>
     <row r="85" spans="1:52">
       <c r="A85" s="30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C85" s="14" t="n">
         <v>1.5</v>
@@ -3340,7 +3394,7 @@
     </row>
     <row r="87" spans="1:52">
       <c r="A87" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B87" s="27" t="s"/>
       <c r="C87" s="28">
@@ -3358,7 +3412,7 @@
     </row>
     <row r="88" spans="1:52">
       <c r="A88" s="27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B88" s="27" t="s"/>
       <c r="C88" s="28">

</xml_diff>

<commit_message>
Stages & Modules decomposition, un-pivot table mode (experimental)
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -725,13 +725,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="40"/>
+    <col customWidth="1" max="1" min="1" style="1" width="50"/>
     <col customWidth="1" hidden="1" max="2" min="2" style="2" width="3"/>
     <col customWidth="1" max="3" min="3" style="1" width="8"/>
-    <col customWidth="1" hidden="1" max="4" min="4" style="3" width="10"/>
-    <col customWidth="1" hidden="1" max="5" min="5" style="3" width="20"/>
-    <col customWidth="1" hidden="1" max="6" min="6" style="3" width="20"/>
-    <col customWidth="1" hidden="1" max="7" min="7" style="3" width="20"/>
+    <col customWidth="1" hidden="1" max="4" min="4" style="3" width="50"/>
+    <col customWidth="1" hidden="1" max="5" min="5" style="3" width="10"/>
+    <col customWidth="1" hidden="1" max="6" min="6" style="3" width="10"/>
+    <col customWidth="1" hidden="1" max="7" min="7" style="3" width="10"/>
     <col customWidth="1" max="8" min="8" style="3" width="50"/>
     <col customWidth="1" max="9" min="9" style="4" width="8"/>
     <col customWidth="1" max="10" min="10" style="4" width="8"/>
@@ -913,7 +913,7 @@
       <c r="K5" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="17">
         <f>TRIM(A5)</f>
         <v/>
       </c>
@@ -980,7 +980,7 @@
       <c r="K7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="17">
         <f>TRIM(A7)</f>
         <v/>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="K9" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="17">
         <f>TRIM(A9)</f>
         <v/>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="K11" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="17">
         <f>TRIM(A11)</f>
         <v/>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="K14" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="17">
         <f>TRIM(A14)</f>
         <v/>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="K16" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="17">
         <f>TRIM(A16)</f>
         <v/>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="K18" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="17">
         <f>TRIM(A18)</f>
         <v/>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="K20" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="17">
         <f>TRIM(A20)</f>
         <v/>
       </c>
@@ -1540,7 +1540,7 @@
       <c r="K24" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="17">
         <f>TRIM(A24)</f>
         <v/>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="K26" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26" s="17">
         <f>TRIM(A26)</f>
         <v/>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="K28" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P28" s="17">
         <f>TRIM(A28)</f>
         <v/>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="K30" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30" s="17">
         <f>TRIM(A30)</f>
         <v/>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="K31" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31" s="17">
         <f>TRIM(A31)</f>
         <v/>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="K33" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P33" s="4">
+      <c r="P33" s="17">
         <f>TRIM(A33)</f>
         <v/>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="K34" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P34" s="4">
+      <c r="P34" s="17">
         <f>TRIM(A34)</f>
         <v/>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="K38" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P38" s="4">
+      <c r="P38" s="17">
         <f>TRIM(A38)</f>
         <v/>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="K40" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P40" s="4">
+      <c r="P40" s="17">
         <f>TRIM(A40)</f>
         <v/>
       </c>
@@ -2123,7 +2123,7 @@
       <c r="K42" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P42" s="4">
+      <c r="P42" s="17">
         <f>TRIM(A42)</f>
         <v/>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="K44" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P44" s="4">
+      <c r="P44" s="17">
         <f>TRIM(A44)</f>
         <v/>
       </c>
@@ -2257,7 +2257,7 @@
       <c r="K46" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P46" s="4">
+      <c r="P46" s="17">
         <f>TRIM(A46)</f>
         <v/>
       </c>
@@ -2326,7 +2326,7 @@
       <c r="K48" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="P48" s="4">
+      <c r="P48" s="17">
         <f>TRIM(A48)</f>
         <v/>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="K51" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="P51" s="4">
+      <c r="P51" s="17">
         <f>TRIM(A51)</f>
         <v/>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="K53" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="P53" s="4">
+      <c r="P53" s="17">
         <f>TRIM(A53)</f>
         <v/>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="K55" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="P55" s="4">
+      <c r="P55" s="17">
         <f>TRIM(A55)</f>
         <v/>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="K65" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="P65" s="4">
+      <c r="P65" s="17">
         <f>TRIM(A65)</f>
         <v/>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="K67" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="P67" s="4">
+      <c r="P67" s="17">
         <f>TRIM(A67)</f>
         <v/>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="K72" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="P72" s="4">
+      <c r="P72" s="17">
         <f>TRIM(A72)</f>
         <v/>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="K76" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="P76" s="4">
+      <c r="P76" s="17">
         <f>TRIM(A76)</f>
         <v/>
       </c>
@@ -3381,6 +3381,10 @@
       </c>
       <c r="C84" s="14">
         <f>SQRT(O78)</f>
+        <v/>
+      </c>
+      <c r="H84" s="29">
+        <f>C84/M78</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Multi-page mode (separate footer + stage-and-roles page)
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.deep.xlsx
+++ b/example/Estimation Tool.mm.deep.xlsx
@@ -717,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ88"/>
+  <dimension ref="A1:AZ89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3247,41 +3247,9 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:52">
-      <c r="A79" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" s="27" t="s"/>
-      <c r="C79" s="27" t="s"/>
-      <c r="D79" s="27" t="s"/>
-      <c r="E79" s="27" t="s"/>
-      <c r="F79" s="27" t="s"/>
-      <c r="G79" s="27" t="s"/>
-      <c r="H79" s="27" t="s"/>
-      <c r="I79" s="28">
-        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
-        <v/>
-      </c>
-      <c r="J79" s="28">
-        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
-        <v/>
-      </c>
-      <c r="K79" s="28">
-        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
-        <v/>
-      </c>
-      <c r="M79" s="28">
-        <f>(I79+4*J79+K79)/6</f>
-        <v/>
-      </c>
-      <c r="N79" s="29">
-        <f>(M79/Estimates!M78)</f>
-        <v/>
-      </c>
-    </row>
     <row r="80" spans="1:52">
       <c r="A80" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" s="27" t="s"/>
       <c r="C80" s="27" t="s"/>
@@ -3291,15 +3259,15 @@
       <c r="G80" s="27" t="s"/>
       <c r="H80" s="27" t="s"/>
       <c r="I80" s="28">
-        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
+        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="J80" s="28">
-        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
+        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="K80" s="28">
-        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
+        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(adm)")</f>
         <v/>
       </c>
       <c r="M80" s="28">
@@ -3310,10 +3278,14 @@
         <f>(M80/Estimates!M78)</f>
         <v/>
       </c>
+      <c r="P80" s="2">
+        <f>IF(N80&gt;0, 1, 0)</f>
+        <v/>
+      </c>
     </row>
     <row r="81" spans="1:52">
       <c r="A81" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" s="27" t="s"/>
       <c r="C81" s="27" t="s"/>
@@ -3323,15 +3295,15 @@
       <c r="G81" s="27" t="s"/>
       <c r="H81" s="27" t="s"/>
       <c r="I81" s="28">
-        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
+        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="J81" s="28">
-        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
+        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="K81" s="28">
-        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
+        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(analysis)")</f>
         <v/>
       </c>
       <c r="M81" s="28">
@@ -3342,10 +3314,14 @@
         <f>(M81/Estimates!M78)</f>
         <v/>
       </c>
+      <c r="P81" s="2">
+        <f>IF(N81&gt;0, 1, 0)</f>
+        <v/>
+      </c>
     </row>
     <row r="82" spans="1:52">
       <c r="A82" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B82" s="27" t="s"/>
       <c r="C82" s="27" t="s"/>
@@ -3355,15 +3331,15 @@
       <c r="G82" s="27" t="s"/>
       <c r="H82" s="27" t="s"/>
       <c r="I82" s="28">
-        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="J82" s="28">
-        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="K82" s="28">
-        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(coding)")</f>
         <v/>
       </c>
       <c r="M82" s="28">
@@ -3374,53 +3350,75 @@
         <f>(M82/Estimates!M78)</f>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:52">
-      <c r="A84" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C84" s="14">
-        <f>SQRT(O78)</f>
-        <v/>
-      </c>
-      <c r="H84" s="31">
-        <f>C84/M78</f>
+      <c r="P82" s="2">
+        <f>IF(N82&gt;0, 1, 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:52">
+      <c r="A83" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="27" t="s"/>
+      <c r="C83" s="27" t="s"/>
+      <c r="D83" s="27" t="s"/>
+      <c r="E83" s="27" t="s"/>
+      <c r="F83" s="27" t="s"/>
+      <c r="G83" s="27" t="s"/>
+      <c r="H83" s="27" t="s"/>
+      <c r="I83" s="28">
+        <f>SUMIFS(Estimates!I2:I77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <v/>
+      </c>
+      <c r="J83" s="28">
+        <f>SUMIFS(Estimates!J2:J77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <v/>
+      </c>
+      <c r="K83" s="28">
+        <f>SUMIFS(Estimates!K2:K77,Estimates!B2:B77,"=0",Estimates!P2:P77,"(test)")</f>
+        <v/>
+      </c>
+      <c r="M83" s="28">
+        <f>(I83+4*J83+K83)/6</f>
+        <v/>
+      </c>
+      <c r="N83" s="29">
+        <f>(M83/Estimates!M78)</f>
+        <v/>
+      </c>
+      <c r="P83" s="2">
+        <f>IF(N83&gt;0, 1, 0)</f>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:52">
       <c r="A85" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C85" s="14">
+        <f>SQRT(O78)</f>
+        <v/>
+      </c>
+      <c r="H85" s="31">
+        <f>C85/M78</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:52">
+      <c r="A86" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C85" s="14" t="n">
+      <c r="C86" s="14" t="n">
         <v>1.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:52">
-      <c r="A87" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="27" t="s"/>
-      <c r="C87" s="28">
-        <f>M78-1*C84</f>
-        <v/>
-      </c>
-      <c r="D87" s="27" t="s"/>
-      <c r="E87" s="27" t="s"/>
-      <c r="F87" s="27" t="s"/>
-      <c r="G87" s="27" t="s"/>
-      <c r="H87" s="32">
-        <f>C87*Estimates!C85</f>
-        <v/>
       </c>
     </row>
     <row r="88" spans="1:52">
       <c r="A88" s="27" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B88" s="27" t="s"/>
       <c r="C88" s="28">
-        <f>M78+2*C84</f>
+        <f>M78-1*C85</f>
         <v/>
       </c>
       <c r="D88" s="27" t="s"/>
@@ -3428,7 +3426,25 @@
       <c r="F88" s="27" t="s"/>
       <c r="G88" s="27" t="s"/>
       <c r="H88" s="32">
-        <f>C88*Estimates!C85</f>
+        <f>C88*Estimates!C86</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:52">
+      <c r="A89" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" s="27" t="s"/>
+      <c r="C89" s="28">
+        <f>M78+2*C85</f>
+        <v/>
+      </c>
+      <c r="D89" s="27" t="s"/>
+      <c r="E89" s="27" t="s"/>
+      <c r="F89" s="27" t="s"/>
+      <c r="G89" s="27" t="s"/>
+      <c r="H89" s="32">
+        <f>C89*Estimates!C86</f>
         <v/>
       </c>
     </row>

</xml_diff>